<commit_message>
add comparision of Tesla and TITAN
</commit_message>
<xml_diff>
--- a/benchmark_neighlist_gpu.xlsx
+++ b/benchmark_neighlist_gpu.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="520" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>GeForce GTX TITAN</t>
   </si>
@@ -41,6 +41,22 @@
   </si>
   <si>
     <t>Tesla K40t</t>
+  </si>
+  <si>
+    <t>without smem (TITAN)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>with smem (TITAN)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>without smem (Tesla)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>with smem (Tesla)</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -213,11 +229,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1011517184"/>
-        <c:axId val="1011519504"/>
+        <c:axId val="1783779312"/>
+        <c:axId val="1824049408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1011517184"/>
+        <c:axId val="1783779312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -257,7 +273,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1011519504"/>
+        <c:crossAx val="1824049408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -265,7 +281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1011519504"/>
+        <c:axId val="1824049408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,7 +410,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1011517184"/>
+        <c:crossAx val="1783779312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -443,6 +459,406 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>without smem (TITAN)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>with smem (TITAN)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>without smem (Tesla)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>with smem (Tesla)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1004.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>857.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2041.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1775.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1827484464"/>
+        <c:axId val="1827500688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1827484464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1827500688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1827500688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP" sz="1800" b="0" i="0" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>100</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US" sz="1800" b="0" i="0" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>回近傍粒子リストを構築するのに要した時間 </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP" sz="1800" b="0" i="0" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>[ms]</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1800">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ja-JP" altLang="en-US">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1827484464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -483,7 +899,552 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1246,7 +2207,622 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>825499</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>778932</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="グラフ 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.49129</cdr:x>
+      <cdr:y>0.45882</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.54776</cdr:x>
+      <cdr:y>0.54861</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="右矢印 1"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="10800000">
+          <a:off x="4419600" y="2476500"/>
+          <a:ext cx="508001" cy="484632"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rtlCol="0" anchor="t"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.75388</cdr:x>
+      <cdr:y>0.08</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.81035</cdr:x>
+      <cdr:y>0.16979</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="右矢印 2"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="10800000">
+          <a:off x="6781800" y="431800"/>
+          <a:ext cx="508001" cy="484632"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rtlCol="0" anchor="t"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.55624</cdr:x>
+      <cdr:y>0.44235</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.68997</cdr:x>
+      <cdr:y>0.56387</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="テキスト ボックス 3"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5003800" y="2387600"/>
+          <a:ext cx="1203086" cy="655885"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600"/>
+            <a:t>x1.17</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.816</cdr:x>
+      <cdr:y>0.06353</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.94974</cdr:x>
+      <cdr:y>0.18505</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="テキスト ボックス 4"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7340600" y="342900"/>
+          <a:ext cx="1203086" cy="655885"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600"/>
+            <a:t>x1.14</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1512,10 +3088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -1563,9 +3139,50 @@
         <v>11.905298759864712</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>857</v>
+      </c>
+      <c r="D7">
+        <f>B6/B7</f>
+        <v>1.1715285880980164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1775</v>
+      </c>
+      <c r="D9">
+        <f>B8/B9</f>
+        <v>1.1498591549295774</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>